<commit_message>
Added feature extraction w/ random forest classification.
</commit_message>
<xml_diff>
--- a/results/accuracy.xlsx
+++ b/results/accuracy.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="133">
   <si>
     <t>Dataset</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>LSTM</t>
+  </si>
+  <si>
+    <t>FEAT_RandForest</t>
   </si>
   <si>
     <t>ACSF1</t>
@@ -767,13 +770,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D129"/>
+  <dimension ref="A1:E129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -786,10 +789,13 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>0.6200000047683716</v>
@@ -798,12 +804,15 @@
         <v>0.6399999856948853</v>
       </c>
       <c r="D2">
-        <v>0.6700000166893005</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>0.6899999976158142</v>
+      </c>
+      <c r="E2">
+        <v>0.8100000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>0.6410256624221802</v>
@@ -812,12 +821,15 @@
         <v>0.6153846383094788</v>
       </c>
       <c r="D3">
-        <v>0.2615384757518768</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.2871794998645782</v>
+      </c>
+      <c r="E3">
+        <v>0.7794871794871795</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>0.4966666698455811</v>
@@ -826,12 +838,15 @@
         <v>0.5833333134651184</v>
       </c>
       <c r="D4">
-        <v>0.5033333301544189</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>0.4600000083446503</v>
+      </c>
+      <c r="E4">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>0.6499999761581421</v>
@@ -842,10 +857,13 @@
       <c r="D5">
         <v>0.6566666960716248</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5">
+        <v>0.7766666666666666</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>0.4799999892711639</v>
@@ -854,12 +872,15 @@
         <v>0.5433333516120911</v>
       </c>
       <c r="D6">
-        <v>0.476666659116745</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>0.4533333480358124</v>
+      </c>
+      <c r="E6">
+        <v>0.6766666666666666</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>0.9166666865348816</v>
@@ -868,12 +889,15 @@
         <v>0.8611111044883728</v>
       </c>
       <c r="D7">
-        <v>0.8611111044883728</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>0.9166666865348816</v>
+      </c>
+      <c r="E7">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>0.5666666626930237</v>
@@ -882,12 +906,15 @@
         <v>0.3666666746139526</v>
       </c>
       <c r="D8">
-        <v>0.6000000238418579</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>0.6333333253860474</v>
+      </c>
+      <c r="E8">
+        <v>0.4666666666666667</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>0.6499999761581421</v>
@@ -896,12 +923,15 @@
         <v>0.550000011920929</v>
       </c>
       <c r="D9">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>0.699999988079071</v>
+      </c>
+      <c r="E9">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>0.800000011920929</v>
@@ -912,10 +942,13 @@
       <c r="D10">
         <v>0.550000011920929</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -924,12 +957,15 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <v>0.9666666388511658</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>0.5833333134651184</v>
@@ -938,12 +974,15 @@
         <v>0.6000000238418579</v>
       </c>
       <c r="D12">
-        <v>0.6833333373069763</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>0.6333333253860474</v>
+      </c>
+      <c r="E12">
+        <v>0.6666666666666666</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -954,10 +993,13 @@
       <c r="D13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -968,10 +1010,13 @@
       <c r="D14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>0.9957173466682434</v>
@@ -982,10 +1027,13 @@
       <c r="D15">
         <v>0.597430408000946</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15">
+        <v>0.9914346895074947</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -996,10 +1044,13 @@
       <c r="D16">
         <v>0.9750000238418579</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>0.5</v>
@@ -1010,10 +1061,13 @@
       <c r="D17">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17">
+        <v>0.9642857142857143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>0.4440000057220459</v>
@@ -1022,12 +1076,15 @@
         <v>0.5759999752044678</v>
       </c>
       <c r="D18">
-        <v>0.6919999718666077</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>0.6240000128746033</v>
+      </c>
+      <c r="E18">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>0.4897435903549194</v>
@@ -1038,10 +1095,13 @@
       <c r="D19">
         <v>0.5871794819831848</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19">
+        <v>0.6307692307692307</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B20">
         <v>0.4743589758872986</v>
@@ -1052,10 +1112,13 @@
       <c r="D20">
         <v>0.5820512771606445</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20">
+        <v>0.5846153846153846</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B21">
         <v>0.5102564096450806</v>
@@ -1066,10 +1129,13 @@
       <c r="D21">
         <v>0.6435897350311279</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21">
+        <v>0.5846153846153846</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B22">
         <v>0.7213888764381409</v>
@@ -1080,10 +1146,13 @@
       <c r="D22">
         <v>0.6491666436195374</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22">
+        <v>0.7926388888888889</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1094,10 +1163,13 @@
       <c r="D23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B24">
         <v>0.8125</v>
@@ -1108,10 +1180,13 @@
       <c r="D24">
         <v>0.8575000166893005</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24">
+        <v>0.835</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B25">
         <v>0.8083333373069763</v>
@@ -1122,10 +1197,13 @@
       <c r="D25">
         <v>0.8299999833106995</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25">
+        <v>0.8100000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B26">
         <v>0.7674999833106995</v>
@@ -1136,10 +1214,13 @@
       <c r="D26">
         <v>0.7850000262260437</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B27">
         <v>0.5641025900840759</v>
@@ -1150,10 +1231,13 @@
       <c r="D27">
         <v>0.5384615659713745</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27">
+        <v>0.5384615384615384</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B28">
         <v>0.8999999761581421</v>
@@ -1164,10 +1248,13 @@
       <c r="D28">
         <v>0.8999999761581421</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -1178,10 +1265,13 @@
       <c r="D29">
         <v>0.8500000238418579</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B30">
         <v>0.8167701959609985</v>
@@ -1192,10 +1282,13 @@
       <c r="D30">
         <v>0.8167701959609985</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30">
+        <v>0.8167701863354038</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B31">
         <v>0.8799999952316284</v>
@@ -1206,10 +1299,13 @@
       <c r="D31">
         <v>0.8999999761581421</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B32">
         <v>0.9620000123977661</v>
@@ -1220,10 +1316,13 @@
       <c r="D32">
         <v>0.9559999704360962</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32">
+        <v>0.954</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -1234,10 +1333,13 @@
       <c r="D33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B34">
         <v>0.567891538143158</v>
@@ -1248,10 +1350,13 @@
       <c r="D34">
         <v>0.6580775380134583</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34">
+        <v>0.7185749495854806</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B35">
         <v>0.3729281723499298</v>
@@ -1262,10 +1367,13 @@
       <c r="D35">
         <v>0.4723756909370422</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35">
+        <v>0.5552486187845304</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B36">
         <v>0.2458563596010208</v>
@@ -1276,10 +1384,13 @@
       <c r="D36">
         <v>0.3204419910907745</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36">
+        <v>0.4668508287292817</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B37">
         <v>0.5892857313156128</v>
@@ -1290,10 +1401,13 @@
       <c r="D37">
         <v>0.3492063581943512</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37">
+        <v>0.3948412698412698</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B38">
         <v>0.8892857432365417</v>
@@ -1304,10 +1418,13 @@
       <c r="D38">
         <v>0.7642857432365417</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38">
+        <v>0.8803571428571428</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B39">
         <v>0.7916666865348816</v>
@@ -1318,10 +1435,13 @@
       <c r="D39">
         <v>0.9166666865348816</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39">
+        <v>0.7916666666666666</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B40">
         <v>0.9750000238418579</v>
@@ -1332,10 +1452,13 @@
       <c r="D40">
         <v>0.9150000214576721</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="E40">
+        <v>0.985</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B41">
         <v>0.6711111068725586</v>
@@ -1346,10 +1469,13 @@
       <c r="D41">
         <v>0.4533333480358124</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="E41">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B42">
         <v>0.8628571629524231</v>
@@ -1360,10 +1486,13 @@
       <c r="D42">
         <v>0.7885714173316956</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="E42">
+        <v>0.8285714285714286</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B43">
         <v>0.7642321586608887</v>
@@ -1374,10 +1503,13 @@
       <c r="D43">
         <v>0.9227992296218872</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="E43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B44">
         <v>0.6256875395774841</v>
@@ -1388,10 +1520,13 @@
       <c r="D44">
         <v>0.9133663177490234</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="E44">
+        <v>0.9276677667766776</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B45">
         <v>0.9933333396911621</v>
@@ -1402,10 +1537,13 @@
       <c r="D45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="E45">
+        <v>0.9933333333333333</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -1416,10 +1554,13 @@
       <c r="D46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="E46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -1430,10 +1571,13 @@
       <c r="D47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
+      <c r="E47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B48">
         <v>0.4423076808452606</v>
@@ -1444,10 +1588,13 @@
       <c r="D48">
         <v>0.4711538553237915</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="E48">
+        <v>0.1538461538461539</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B49">
         <v>0.5240384340286255</v>
@@ -1458,10 +1605,13 @@
       <c r="D49">
         <v>0.4134615361690521</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="E49">
+        <v>0.5769230769230769</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B50">
         <v>0.3076923191547394</v>
@@ -1472,10 +1622,13 @@
       <c r="D50">
         <v>0.2355769276618958</v>
       </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="E50">
+        <v>0.1057692307692308</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B51">
         <v>0.810606062412262</v>
@@ -1486,10 +1639,13 @@
       <c r="D51">
         <v>0.8409090638160706</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="E51">
+        <v>0.8484848484848485</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B52">
         <v>0.568493127822876</v>
@@ -1500,10 +1656,13 @@
       <c r="D52">
         <v>0.7534246444702148</v>
       </c>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="E52">
+        <v>0.7602739726027398</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B53">
         <v>0.9399999976158142</v>
@@ -1514,10 +1673,13 @@
       <c r="D53">
         <v>0.9599999785423279</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
+      <c r="E53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B54">
         <v>0.9111111164093018</v>
@@ -1528,10 +1690,13 @@
       <c r="D54">
         <v>0.9555555582046509</v>
       </c>
-    </row>
-    <row r="55" spans="1:4">
+      <c r="E54">
+        <v>0.9925925925925926</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -1542,10 +1707,13 @@
       <c r="D55">
         <v>0.9925925731658936</v>
       </c>
-    </row>
-    <row r="56" spans="1:4">
+      <c r="E55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -1556,10 +1724,13 @@
       <c r="D56">
         <v>0.9926470518112183</v>
       </c>
-    </row>
-    <row r="57" spans="1:4">
+      <c r="E56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B57">
         <v>0.6972476840019226</v>
@@ -1570,10 +1741,13 @@
       <c r="D57">
         <v>0.6697247624397278</v>
       </c>
-    </row>
-    <row r="58" spans="1:4">
+      <c r="E57">
+        <v>0.6697247706422018</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B58">
         <v>0.8410000205039978</v>
@@ -1584,10 +1758,13 @@
       <c r="D58">
         <v>0.8659999966621399</v>
       </c>
-    </row>
-    <row r="59" spans="1:4">
+      <c r="E58">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B59">
         <v>0.5548387169837952</v>
@@ -1598,10 +1775,13 @@
       <c r="D59">
         <v>0.5870967507362366</v>
       </c>
-    </row>
-    <row r="60" spans="1:4">
+      <c r="E59">
+        <v>0.5548387096774193</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B60">
         <v>0.578125</v>
@@ -1612,10 +1792,13 @@
       <c r="D60">
         <v>0.578125</v>
       </c>
-    </row>
-    <row r="61" spans="1:4">
+      <c r="E60">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B61">
         <v>0.800000011920929</v>
@@ -1626,10 +1809,13 @@
       <c r="D61">
         <v>0.8999999761581421</v>
       </c>
-    </row>
-    <row r="62" spans="1:4">
+      <c r="E61">
+        <v>0.975</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B62">
         <v>0.4300000071525574</v>
@@ -1640,10 +1826,13 @@
       <c r="D62">
         <v>0.550000011920929</v>
       </c>
-    </row>
-    <row r="63" spans="1:4">
+      <c r="E62">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B63">
         <v>0.8870967626571655</v>
@@ -1654,10 +1843,13 @@
       <c r="D63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:4">
+      <c r="E63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -1668,10 +1860,13 @@
       <c r="D64">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:4">
+      <c r="E64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B65">
         <v>0.6863636374473572</v>
@@ -1682,10 +1877,13 @@
       <c r="D65">
         <v>0.6954545378684998</v>
       </c>
-    </row>
-    <row r="66" spans="1:4">
+      <c r="E65">
+        <v>0.6954545454545454</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B66">
         <v>0.9850746393203735</v>
@@ -1696,10 +1894,13 @@
       <c r="D66">
         <v>0.9701492786407471</v>
       </c>
-    </row>
-    <row r="67" spans="1:4">
+      <c r="E66">
+        <v>0.9850746268656716</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B67">
         <v>0.3946666717529297</v>
@@ -1710,10 +1911,13 @@
       <c r="D67">
         <v>0.7866666913032532</v>
       </c>
-    </row>
-    <row r="68" spans="1:4">
+      <c r="E67">
+        <v>0.8106666666666666</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B68">
         <v>0.7666666507720947</v>
@@ -1724,10 +1928,13 @@
       <c r="D68">
         <v>0.800000011920929</v>
       </c>
-    </row>
-    <row r="69" spans="1:4">
+      <c r="E68">
+        <v>0.8666666666666667</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B69">
         <v>0.5428571701049805</v>
@@ -1738,10 +1945,13 @@
       <c r="D69">
         <v>0.6571428775787354</v>
       </c>
-    </row>
-    <row r="70" spans="1:4">
+      <c r="E69">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B70">
         <v>0.9818181991577148</v>
@@ -1752,10 +1962,13 @@
       <c r="D70">
         <v>0.9636363387107849</v>
       </c>
-    </row>
-    <row r="71" spans="1:4">
+      <c r="E70">
+        <v>0.9636363636363636</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
       <c r="A71" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B71">
         <v>0.3333333432674408</v>
@@ -1766,10 +1979,13 @@
       <c r="D71">
         <v>0.6666666865348816</v>
       </c>
-    </row>
-    <row r="72" spans="1:4">
+      <c r="E71">
+        <v>0.9333333333333333</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
       <c r="A72" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B72">
         <v>0.7191600799560547</v>
@@ -1780,10 +1996,13 @@
       <c r="D72">
         <v>0.6771653294563293</v>
       </c>
-    </row>
-    <row r="73" spans="1:4">
+      <c r="E72">
+        <v>0.800524934383202</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B73">
         <v>0.9137353301048279</v>
@@ -1794,10 +2013,13 @@
       <c r="D73">
         <v>0.8819095492362976</v>
       </c>
-    </row>
-    <row r="74" spans="1:4">
+      <c r="E73">
+        <v>0.9530988274706867</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
       <c r="A74" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B74">
         <v>0.7549999952316284</v>
@@ -1808,10 +2030,13 @@
       <c r="D74">
         <v>0.8100000023841858</v>
       </c>
-    </row>
-    <row r="75" spans="1:4">
+      <c r="E74">
+        <v>0.7725</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
       <c r="A75" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B75">
         <v>0.596666693687439</v>
@@ -1822,10 +2047,13 @@
       <c r="D75">
         <v>0.5866666436195374</v>
       </c>
-    </row>
-    <row r="76" spans="1:4">
+      <c r="E75">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
       <c r="A76" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B76">
         <v>0.6190476417541504</v>
@@ -1836,10 +2064,13 @@
       <c r="D76">
         <v>0.6365914940834045</v>
       </c>
-    </row>
-    <row r="77" spans="1:4">
+      <c r="E76">
+        <v>0.6466165413533834</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
       <c r="A77" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B77">
         <v>0.9520000219345093</v>
@@ -1850,10 +2081,13 @@
       <c r="D77">
         <v>0.9639999866485596</v>
       </c>
-    </row>
-    <row r="78" spans="1:4">
+      <c r="E77">
+        <v>0.968</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
       <c r="A78" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B78">
         <v>0.9900000095367432</v>
@@ -1864,10 +2098,13 @@
       <c r="D78">
         <v>0.9900000095367432</v>
       </c>
-    </row>
-    <row r="79" spans="1:4">
+      <c r="E78">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
       <c r="A79" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B79">
         <v>0.949999988079071</v>
@@ -1878,10 +2115,13 @@
       <c r="D79">
         <v>0.949999988079071</v>
       </c>
-    </row>
-    <row r="80" spans="1:4">
+      <c r="E79">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
       <c r="A80" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B80">
         <v>0.8777777552604675</v>
@@ -1892,10 +2132,13 @@
       <c r="D80">
         <v>0.5577777624130249</v>
       </c>
-    </row>
-    <row r="81" spans="1:4">
+      <c r="E80">
+        <v>0.8911111111111111</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B81">
         <v>0.9111111164093018</v>
@@ -1906,10 +2149,13 @@
       <c r="D81">
         <v>0.6366666555404663</v>
       </c>
-    </row>
-    <row r="82" spans="1:4">
+      <c r="E81">
+        <v>0.8994444444444445</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B82">
         <v>0.5333333611488342</v>
@@ -1920,10 +2166,13 @@
       <c r="D82">
         <v>0.4333333373069763</v>
       </c>
-    </row>
-    <row r="83" spans="1:4">
+      <c r="E82">
+        <v>0.9333333333333333</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B83">
         <v>0.6050000190734863</v>
@@ -1934,10 +2183,13 @@
       <c r="D83">
         <v>0.8349999785423279</v>
       </c>
-    </row>
-    <row r="84" spans="1:4">
+      <c r="E83">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B84">
         <v>0.7649999856948853</v>
@@ -1948,10 +2200,13 @@
       <c r="D84">
         <v>0.6449999809265137</v>
       </c>
-    </row>
-    <row r="85" spans="1:4">
+      <c r="E84">
+        <v>0.8011111111111111</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B85">
         <v>0.1542056053876877</v>
@@ -1962,10 +2217,13 @@
       <c r="D85">
         <v>0.3271028101444244</v>
       </c>
-    </row>
-    <row r="86" spans="1:4">
+      <c r="E85">
+        <v>0.4813084112149533</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B86">
         <v>0.699999988079071</v>
@@ -1976,10 +2234,13 @@
       <c r="D86">
         <v>0.8600000143051147</v>
       </c>
-    </row>
-    <row r="87" spans="1:4">
+      <c r="E86">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B87">
         <v>0.05769230797886848</v>
@@ -1990,10 +2251,13 @@
       <c r="D87">
         <v>0.1057692319154739</v>
       </c>
-    </row>
-    <row r="88" spans="1:4">
+      <c r="E87">
+        <v>0.7307692307692307</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B88">
         <v>0.25</v>
@@ -2004,10 +2268,13 @@
       <c r="D88">
         <v>0.3653846085071564</v>
       </c>
-    </row>
-    <row r="89" spans="1:4">
+      <c r="E88">
+        <v>0.9519230769230769</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B89">
         <v>0.115384615957737</v>
@@ -2018,10 +2285,13 @@
       <c r="D89">
         <v>0.1826923042535782</v>
       </c>
-    </row>
-    <row r="90" spans="1:4">
+      <c r="E89">
+        <v>0.9519230769230769</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B90">
         <v>0.3240223526954651</v>
@@ -2032,10 +2302,13 @@
       <c r="D90">
         <v>0.3780260682106018</v>
       </c>
-    </row>
-    <row r="91" spans="1:4">
+      <c r="E90">
+        <v>0.8938547486033519</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B91">
         <v>0.9523809552192688</v>
@@ -2046,10 +2319,13 @@
       <c r="D91">
         <v>0.9809523820877075</v>
       </c>
-    </row>
-    <row r="92" spans="1:4">
+      <c r="E91">
+        <v>0.9904761904761905</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
       <c r="A92" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B92">
         <v>0.9833333492279053</v>
@@ -2060,10 +2336,13 @@
       <c r="D92">
         <v>0.9333333373069763</v>
       </c>
-    </row>
-    <row r="93" spans="1:4">
+      <c r="E92">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
       <c r="A93" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B93">
         <v>0.7549999952316284</v>
@@ -2074,10 +2353,13 @@
       <c r="D93">
         <v>0.7774999737739563</v>
       </c>
-    </row>
-    <row r="94" spans="1:4">
+      <c r="E93">
+        <v>0.805</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
       <c r="A94" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B94">
         <v>0.8033333420753479</v>
@@ -2088,10 +2370,13 @@
       <c r="D94">
         <v>0.7749999761581421</v>
       </c>
-    </row>
-    <row r="95" spans="1:4">
+      <c r="E94">
+        <v>0.8183333333333334</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
       <c r="A95" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B95">
         <v>0.7975000143051147</v>
@@ -2102,10 +2387,13 @@
       <c r="D95">
         <v>0.7799999713897705</v>
       </c>
-    </row>
-    <row r="96" spans="1:4">
+      <c r="E95">
+        <v>0.8100000000000001</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
       <c r="A96" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B96">
         <v>0.3386666774749756</v>
@@ -2116,10 +2404,13 @@
       <c r="D96">
         <v>0.5360000133514404</v>
       </c>
-    </row>
-    <row r="97" spans="1:4">
+      <c r="E96">
+        <v>0.5786666666666667</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
       <c r="A97" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B97">
         <v>0.8500000238418579</v>
@@ -2130,10 +2421,13 @@
       <c r="D97">
         <v>0.6000000238418579</v>
       </c>
-    </row>
-    <row r="98" spans="1:4">
+      <c r="E97">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
       <c r="A98" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B98">
         <v>0.4213333427906036</v>
@@ -2144,10 +2438,13 @@
       <c r="D98">
         <v>0.5013333559036255</v>
       </c>
-    </row>
-    <row r="99" spans="1:4">
+      <c r="E98">
+        <v>0.5093333333333333</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
       <c r="A99" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B99">
         <v>0.95333331823349</v>
@@ -2158,10 +2455,13 @@
       <c r="D99">
         <v>0.79666668176651</v>
       </c>
-    </row>
-    <row r="100" spans="1:4">
+      <c r="E99">
+        <v>0.9266666666666666</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
       <c r="A100" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B100">
         <v>0.5755555629730225</v>
@@ -2172,10 +2472,13 @@
       <c r="D100">
         <v>0.5733333230018616</v>
       </c>
-    </row>
-    <row r="101" spans="1:4">
+      <c r="E100">
+        <v>0.8177777777777778</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
       <c r="A101" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B101">
         <v>0.804444432258606</v>
@@ -2186,10 +2489,13 @@
       <c r="D101">
         <v>0.6666666865348816</v>
       </c>
-    </row>
-    <row r="102" spans="1:4">
+      <c r="E101">
+        <v>0.9422222222222222</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
       <c r="A102" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B102">
         <v>0.5</v>
@@ -2200,10 +2506,13 @@
       <c r="D102">
         <v>0.6200000047683716</v>
       </c>
-    </row>
-    <row r="103" spans="1:4">
+      <c r="E102">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
       <c r="A103" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B103">
         <v>0.4000000059604645</v>
@@ -2214,10 +2523,13 @@
       <c r="D103">
         <v>0.8999999761581421</v>
       </c>
-    </row>
-    <row r="104" spans="1:4">
+      <c r="E103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
       <c r="A104" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B104">
         <v>0.7166666388511658</v>
@@ -2228,10 +2540,13 @@
       <c r="D104">
         <v>0.6633333563804626</v>
       </c>
-    </row>
-    <row r="105" spans="1:4">
+      <c r="E104">
+        <v>0.7483333333333333</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
       <c r="A105" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B105">
         <v>0.3973333239555359</v>
@@ -2242,10 +2557,13 @@
       <c r="D105">
         <v>0.7599999904632568</v>
       </c>
-    </row>
-    <row r="106" spans="1:4">
+      <c r="E105">
+        <v>0.7786666666666666</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
       <c r="A106" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B106">
         <v>0.8799999952316284</v>
@@ -2256,10 +2574,13 @@
       <c r="D106">
         <v>0.9200000166893005</v>
       </c>
-    </row>
-    <row r="107" spans="1:4">
+      <c r="E106">
+        <v>0.9533333333333334</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
       <c r="A107" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B107">
         <v>0.949999988079071</v>
@@ -2270,10 +2591,13 @@
       <c r="D107">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:4">
+      <c r="E107">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
       <c r="A108" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B108">
         <v>1</v>
@@ -2284,10 +2608,13 @@
       <c r="D108">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:4">
+      <c r="E108">
+        <v>0.9629629629629629</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
       <c r="A109" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B109">
         <v>0.9580000042915344</v>
@@ -2298,10 +2625,13 @@
       <c r="D109">
         <v>0.9750000238418579</v>
       </c>
-    </row>
-    <row r="110" spans="1:4">
+      <c r="E109">
+        <v>0.981</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
       <c r="A110" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B110">
         <v>0.9477977156639099</v>
@@ -2312,10 +2642,13 @@
       <c r="D110">
         <v>0.9184339046478271</v>
       </c>
-    </row>
-    <row r="111" spans="1:4">
+      <c r="E110">
+        <v>0.9314845024469821</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
       <c r="A111" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B111">
         <v>0.8679999709129333</v>
@@ -2326,10 +2659,13 @@
       <c r="D111">
         <v>0.8640000224113464</v>
       </c>
-    </row>
-    <row r="112" spans="1:4">
+      <c r="E111">
+        <v>0.952</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
       <c r="A112" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B112">
         <v>0.9599999785423279</v>
@@ -2340,10 +2676,13 @@
       <c r="D112">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:4">
+      <c r="E112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
       <c r="A113" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B113">
         <v>0.9599999785423279</v>
@@ -2354,10 +2693,13 @@
       <c r="D113">
         <v>0.9766666889190674</v>
       </c>
-    </row>
-    <row r="114" spans="1:4">
+      <c r="E113">
+        <v>0.9966666666666667</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
       <c r="A114" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B114">
         <v>0.699999988079071</v>
@@ -2368,10 +2710,13 @@
       <c r="D114">
         <v>0.949999988079071</v>
       </c>
-    </row>
-    <row r="115" spans="1:4">
+      <c r="E114">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
       <c r="A115" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B115">
         <v>0.5833333134651184</v>
@@ -2382,10 +2727,13 @@
       <c r="D115">
         <v>0.6111111044883728</v>
       </c>
-    </row>
-    <row r="116" spans="1:4">
+      <c r="E115">
+        <v>0.7777777777777778</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
       <c r="A116" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B116">
         <v>0.8100000023841858</v>
@@ -2396,10 +2744,13 @@
       <c r="D116">
         <v>0.9700000286102295</v>
       </c>
-    </row>
-    <row r="117" spans="1:4">
+      <c r="E116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
       <c r="A117" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B117">
         <v>1</v>
@@ -2410,10 +2761,13 @@
       <c r="D117">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:4">
+      <c r="E117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
       <c r="A118" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B118">
         <v>0.9649999737739563</v>
@@ -2424,10 +2778,13 @@
       <c r="D118">
         <v>0.9959999918937683</v>
       </c>
-    </row>
-    <row r="119" spans="1:4">
+      <c r="E118">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
       <c r="A119" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B119">
         <v>0.9166666865348816</v>
@@ -2438,10 +2795,13 @@
       <c r="D119">
         <v>0.9722222089767456</v>
       </c>
-    </row>
-    <row r="120" spans="1:4">
+      <c r="E119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
       <c r="A120" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B120">
         <v>0.9776785969734192</v>
@@ -2452,10 +2812,13 @@
       <c r="D120">
         <v>0.9598214030265808</v>
       </c>
-    </row>
-    <row r="121" spans="1:4">
+      <c r="E120">
+        <v>0.9754464285714286</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
       <c r="A121" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B121">
         <v>0.796875</v>
@@ -2466,10 +2829,13 @@
       <c r="D121">
         <v>0.8013392686843872</v>
       </c>
-    </row>
-    <row r="122" spans="1:4">
+      <c r="E121">
+        <v>0.7890625</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
       <c r="A122" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B122">
         <v>0.7544642686843872</v>
@@ -2480,10 +2846,13 @@
       <c r="D122">
         <v>0.7544642686843872</v>
       </c>
-    </row>
-    <row r="123" spans="1:4">
+      <c r="E122">
+        <v>0.7935267857142857</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
       <c r="A123" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B123">
         <v>0.7276785969734192</v>
@@ -2494,10 +2863,13 @@
       <c r="D123">
         <v>0.7611607313156128</v>
       </c>
-    </row>
-    <row r="124" spans="1:4">
+      <c r="E123">
+        <v>0.8035714285714286</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
       <c r="A124" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B124">
         <v>0.9940000176429749</v>
@@ -2508,10 +2880,13 @@
       <c r="D124">
         <v>0.996999979019165</v>
       </c>
-    </row>
-    <row r="125" spans="1:4">
+      <c r="E124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
       <c r="A125" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B125">
         <v>0.4736842215061188</v>
@@ -2522,10 +2897,13 @@
       <c r="D125">
         <v>0.4736842215061188</v>
       </c>
-    </row>
-    <row r="126" spans="1:4">
+      <c r="E125">
+        <v>0.543859649122807</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
       <c r="A126" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B126">
         <v>0.7265917658805847</v>
@@ -2536,10 +2914,13 @@
       <c r="D126">
         <v>0.5393258333206177</v>
       </c>
-    </row>
-    <row r="127" spans="1:4">
+      <c r="E126">
+        <v>0.6816479400749064</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
       <c r="A127" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B127">
         <v>0.4254143536090851</v>
@@ -2550,10 +2931,13 @@
       <c r="D127">
         <v>0.5082873106002808</v>
       </c>
-    </row>
-    <row r="128" spans="1:4">
+      <c r="E127">
+        <v>0.5193370165745856</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
       <c r="A128" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B128">
         <v>0.5524861812591553</v>
@@ -2564,10 +2948,13 @@
       <c r="D128">
         <v>0.5966851115226746</v>
       </c>
-    </row>
-    <row r="129" spans="1:4">
+      <c r="E128">
+        <v>0.6464088397790055</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
       <c r="A129" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B129">
         <v>0.8633333444595337</v>
@@ -2577,6 +2964,9 @@
       </c>
       <c r="D129">
         <v>0.8666666746139526</v>
+      </c>
+      <c r="E129">
+        <v>0.9366666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>